<commit_message>
update domain to www.weiyingjun.top
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="493">
   <si>
     <t>id</t>
   </si>
@@ -1488,6 +1488,24 @@
   </si>
   <si>
     <t>https://pan.quark.cn/s/d314b8afab24</t>
+  </si>
+  <si>
+    <t>病娇男孩的精分日记</t>
+  </si>
+  <si>
+    <t>https://pan.quark.cn/s/992407d06077</t>
+  </si>
+  <si>
+    <t>桔梗物语</t>
+  </si>
+  <si>
+    <t>https://pan.quark.cn/s/be629be38438</t>
+  </si>
+  <si>
+    <t>桐花中路私立协济医院怪谈</t>
+  </si>
+  <si>
+    <t>https://pan.quark.cn/s/3acf12cb40ce</t>
   </si>
 </sst>
 </file>
@@ -2490,10 +2508,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="D208" sqref="D208"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -5413,6 +5431,48 @@
       </c>
       <c r="D208" s="1" t="s">
         <v>486</v>
+      </c>
+    </row>
+    <row r="209" ht="15.5" spans="1:4">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>487</v>
+      </c>
+      <c r="C209" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="210" ht="15.5" spans="1:4">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>489</v>
+      </c>
+      <c r="C210" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="211" ht="15.5" spans="1:4">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>491</v>
+      </c>
+      <c r="C211" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add _headers for ads.txt no-cache
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -3460,9 +3460,9 @@
   <dimension ref="A1:E345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A314" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D346" sqref="D346"/>
+      <selection pane="bottomLeft" activeCell="C344" sqref="C344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>

</xml_diff>